<commit_message>
Wind power generation in China from 2005 to 2019
</commit_message>
<xml_diff>
--- a/figures/123.xlsx
+++ b/figures/123.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joey\Desktop\Swarm2020\Misaka-Conference\figures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Swarm2020\Misaka-Conference\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0463C52-2252-46CD-A7F4-1855F97843A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFCD4FCF-571E-41A0-8AC3-5F561C8660F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" activeTab="2" xr2:uid="{20ABBAC7-A43D-4CA0-B757-679FB53C2F38}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" activeTab="3" xr2:uid="{20ABBAC7-A43D-4CA0-B757-679FB53C2F38}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,12 +28,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>date</t>
   </si>
   <si>
     <t>COVID-19 total confirmed cases worldwide</t>
+  </si>
+  <si>
+    <t>Production (GWh)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wind power generation in China (TWh)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -40,20 +49,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.00_ "/>
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -102,7 +111,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -118,14 +127,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -143,7 +155,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -506,7 +518,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1286643759"/>
@@ -562,7 +574,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1297253951"/>
@@ -604,7 +616,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -641,7 +653,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -655,7 +667,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -998,7 +1010,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1593871103"/>
@@ -1040,7 +1052,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1604918223"/>
@@ -1082,7 +1094,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1119,7 +1131,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1133,7 +1145,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1445,7 +1457,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2106947056"/>
@@ -1487,7 +1499,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="69409904"/>
@@ -1529,7 +1541,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1566,7 +1578,364 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Wind power generation in China (TWh)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="flat" cmpd="dbl" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="34925" cap="flat" cmpd="dbl" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                    <a:alpha val="70000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet4!$A$2:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2019</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet4!$C$2:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.927</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6749999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.71</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44.622</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>74.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>134.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>153.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>186.3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>241</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>305.7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>366</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>405.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C39E-4B12-AB2D-A1E0EF45D07E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="854291567"/>
+        <c:axId val="724373135"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="854291567"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="724373135"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="724373135"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="854291567"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1694,6 +2063,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="343">
   <cs:axisTitle>
@@ -2713,6 +3122,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="243">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="flat" cmpd="dbl" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="flat" cmpd="dbl" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+            <a:alpha val="70000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="2000" kern="1200" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="rnd" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="0" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="243">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3351,8 +4276,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>7143</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>4416</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="图表 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F61E652-BA4B-4319-9EBA-482B2B9DF3E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3654,9 +4620,9 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B1">
         <v>1</v>
       </c>
@@ -3667,7 +4633,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3681,7 +4647,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3695,7 +4661,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3709,7 +4675,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3723,7 +4689,7 @@
         <v>1.875</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3737,7 +4703,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3752,7 +4718,7 @@
       </c>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3767,7 +4733,7 @@
       </c>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3782,7 +4748,7 @@
       </c>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3797,7 +4763,7 @@
       </c>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3812,7 +4778,7 @@
       </c>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3827,130 +4793,130 @@
       </c>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="13:13">
+    <row r="17" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="13:13">
+    <row r="18" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="13:13">
+    <row r="19" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M19" s="4"/>
     </row>
-    <row r="20" spans="13:13">
+    <row r="20" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="13:13">
+    <row r="21" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="13:13">
+    <row r="22" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="13:13">
+    <row r="23" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="13:13">
+    <row r="24" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M24" s="1"/>
     </row>
-    <row r="25" spans="13:13">
+    <row r="25" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="13:13">
+    <row r="26" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M26" s="1"/>
     </row>
-    <row r="27" spans="13:13">
+    <row r="27" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="13:13">
+    <row r="28" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="13:13">
+    <row r="29" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="13:13">
+    <row r="30" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="13:13">
+    <row r="31" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="13:13">
+    <row r="32" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M32" s="1"/>
     </row>
-    <row r="33" spans="13:13">
+    <row r="33" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M33" s="1"/>
     </row>
-    <row r="34" spans="13:13">
+    <row r="34" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M34" s="1"/>
     </row>
-    <row r="35" spans="13:13">
+    <row r="35" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M35" s="1"/>
     </row>
-    <row r="36" spans="13:13">
+    <row r="36" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="13:13">
+    <row r="37" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M37" s="1"/>
     </row>
-    <row r="38" spans="13:13">
+    <row r="38" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M38" s="1"/>
     </row>
-    <row r="39" spans="13:13">
+    <row r="39" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M39" s="1"/>
     </row>
-    <row r="40" spans="13:13">
+    <row r="40" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M40" s="1"/>
     </row>
-    <row r="41" spans="13:13">
+    <row r="41" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M41" s="1"/>
     </row>
-    <row r="42" spans="13:13">
+    <row r="42" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M42" s="1"/>
     </row>
-    <row r="43" spans="13:13">
+    <row r="43" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M43" s="1"/>
     </row>
-    <row r="44" spans="13:13">
+    <row r="44" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M44" s="1"/>
     </row>
-    <row r="45" spans="13:13">
+    <row r="45" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M45" s="1"/>
     </row>
-    <row r="46" spans="13:13">
+    <row r="46" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M46" s="1"/>
     </row>
-    <row r="47" spans="13:13">
+    <row r="47" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M47" s="1"/>
     </row>
-    <row r="48" spans="13:13">
+    <row r="48" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M48" s="1"/>
     </row>
-    <row r="49" spans="13:13">
+    <row r="49" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M49" s="1"/>
     </row>
-    <row r="50" spans="13:13">
+    <row r="50" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M50" s="1"/>
     </row>
-    <row r="51" spans="13:13">
+    <row r="51" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M51" s="1"/>
     </row>
-    <row r="52" spans="13:13">
+    <row r="52" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M52" s="1"/>
     </row>
-    <row r="53" spans="13:13">
+    <row r="53" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M53" s="1"/>
     </row>
-    <row r="54" spans="13:13">
+    <row r="54" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M54" s="1"/>
     </row>
   </sheetData>
@@ -3966,12 +4932,12 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="G1" sqref="G1:G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1">
         <v>0</v>
       </c>
@@ -3988,7 +4954,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4005,7 +4971,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4022,7 +4988,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4039,7 +5005,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4056,7 +5022,7 @@
         <v>2.6666666666999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4073,7 +5039,7 @@
         <v>2.5763888889</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4090,7 +5056,7 @@
         <v>2.5046296296000001</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4107,7 +5073,7 @@
         <v>2.4720293209999999</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4124,7 +5090,7 @@
         <v>2.4634773662999998</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4141,7 +5107,7 @@
         <v>2.4609642917999999</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4158,7 +5124,7 @@
         <v>2.4583583390000001</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4186,16 +5152,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{955944B0-10F1-4623-8085-C475C344F4CE}">
   <dimension ref="A1:B127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -4203,7 +5169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="7">
         <v>43830</v>
       </c>
@@ -4211,7 +5177,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="7">
         <v>43831</v>
       </c>
@@ -4219,7 +5185,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="7">
         <v>43832</v>
       </c>
@@ -4227,7 +5193,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="7">
         <v>43833</v>
       </c>
@@ -4235,7 +5201,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" s="7">
         <v>43834</v>
       </c>
@@ -4243,7 +5209,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" s="7">
         <v>43835</v>
       </c>
@@ -4251,7 +5217,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" s="7">
         <v>43836</v>
       </c>
@@ -4259,7 +5225,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" s="7">
         <v>43837</v>
       </c>
@@ -4267,7 +5233,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" s="7">
         <v>43838</v>
       </c>
@@ -4275,7 +5241,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" s="7">
         <v>43839</v>
       </c>
@@ -4283,7 +5249,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12" s="7">
         <v>43840</v>
       </c>
@@ -4291,7 +5257,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" s="7">
         <v>43841</v>
       </c>
@@ -4299,7 +5265,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" s="7">
         <v>43842</v>
       </c>
@@ -4307,7 +5273,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A15" s="7">
         <v>43843</v>
       </c>
@@ -4315,7 +5281,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A16" s="7">
         <v>43844</v>
       </c>
@@ -4323,7 +5289,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" s="7">
         <v>43845</v>
       </c>
@@ -4331,7 +5297,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A18" s="7">
         <v>43846</v>
       </c>
@@ -4339,7 +5305,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A19" s="7">
         <v>43847</v>
       </c>
@@ -4347,7 +5313,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A20" s="7">
         <v>43848</v>
       </c>
@@ -4355,7 +5321,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A21" s="7">
         <v>43849</v>
       </c>
@@ -4363,7 +5329,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A22" s="7">
         <v>43850</v>
       </c>
@@ -4371,7 +5337,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A23" s="7">
         <v>43851</v>
       </c>
@@ -4379,7 +5345,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A24" s="7">
         <v>43852</v>
       </c>
@@ -4387,7 +5353,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A25" s="7">
         <v>43853</v>
       </c>
@@ -4395,7 +5361,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A26" s="7">
         <v>43854</v>
       </c>
@@ -4403,7 +5369,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A27" s="7">
         <v>43855</v>
       </c>
@@ -4411,7 +5377,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A28" s="7">
         <v>43856</v>
       </c>
@@ -4419,7 +5385,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A29" s="7">
         <v>43857</v>
       </c>
@@ -4427,7 +5393,7 @@
         <v>2820</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A30" s="7">
         <v>43858</v>
       </c>
@@ -4435,7 +5401,7 @@
         <v>4587</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A31" s="7">
         <v>43859</v>
       </c>
@@ -4443,7 +5409,7 @@
         <v>6067</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A32" s="7">
         <v>43860</v>
       </c>
@@ -4451,7 +5417,7 @@
         <v>7823</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A33" s="7">
         <v>43861</v>
       </c>
@@ -4459,7 +5425,7 @@
         <v>9826</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A34" s="7">
         <v>43862</v>
       </c>
@@ -4467,7 +5433,7 @@
         <v>11946</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A35" s="7">
         <v>43863</v>
       </c>
@@ -4475,7 +5441,7 @@
         <v>14554</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A36" s="7">
         <v>43864</v>
       </c>
@@ -4483,7 +5449,7 @@
         <v>17372</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A37" s="7">
         <v>43865</v>
       </c>
@@ -4491,7 +5457,7 @@
         <v>20615</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A38" s="7">
         <v>43866</v>
       </c>
@@ -4499,7 +5465,7 @@
         <v>24522</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A39" s="7">
         <v>43867</v>
       </c>
@@ -4507,7 +5473,7 @@
         <v>28273</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A40" s="7">
         <v>43868</v>
       </c>
@@ -4515,7 +5481,7 @@
         <v>31491</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A41" s="7">
         <v>43869</v>
       </c>
@@ -4523,7 +5489,7 @@
         <v>34933</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A42" s="7">
         <v>43870</v>
       </c>
@@ -4531,7 +5497,7 @@
         <v>37552</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A43" s="7">
         <v>43871</v>
       </c>
@@ -4539,7 +5505,7 @@
         <v>40540</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A44" s="7">
         <v>43872</v>
       </c>
@@ -4547,7 +5513,7 @@
         <v>43105</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A45" s="7">
         <v>43873</v>
       </c>
@@ -4555,7 +5521,7 @@
         <v>45177</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A46" s="7">
         <v>43874</v>
       </c>
@@ -4563,7 +5529,7 @@
         <v>60328</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A47" s="7">
         <v>43875</v>
       </c>
@@ -4571,7 +5537,7 @@
         <v>64543</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A48" s="7">
         <v>43876</v>
       </c>
@@ -4579,7 +5545,7 @@
         <v>67103</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A49" s="7">
         <v>43877</v>
       </c>
@@ -4587,7 +5553,7 @@
         <v>69265</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A50" s="7">
         <v>43878</v>
       </c>
@@ -4595,7 +5561,7 @@
         <v>71332</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A51" s="7">
         <v>43879</v>
       </c>
@@ -4603,7 +5569,7 @@
         <v>73327</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A52" s="7">
         <v>43880</v>
       </c>
@@ -4611,7 +5577,7 @@
         <v>75191</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A53" s="7">
         <v>43881</v>
       </c>
@@ -4619,7 +5585,7 @@
         <v>75723</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A54" s="7">
         <v>43882</v>
       </c>
@@ -4627,7 +5593,7 @@
         <v>76719</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A55" s="7">
         <v>43883</v>
       </c>
@@ -4635,7 +5601,7 @@
         <v>77804</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A56" s="7">
         <v>43884</v>
       </c>
@@ -4643,7 +5609,7 @@
         <v>78812</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A57" s="7">
         <v>43885</v>
       </c>
@@ -4651,7 +5617,7 @@
         <v>79339</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A58" s="7">
         <v>43886</v>
       </c>
@@ -4659,7 +5625,7 @@
         <v>80132</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A59" s="7">
         <v>43887</v>
       </c>
@@ -4667,7 +5633,7 @@
         <v>80995</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A60" s="7">
         <v>43888</v>
       </c>
@@ -4675,7 +5641,7 @@
         <v>82101</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A61" s="7">
         <v>43889</v>
       </c>
@@ -4683,7 +5649,7 @@
         <v>83365</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A62" s="7">
         <v>43890</v>
       </c>
@@ -4691,7 +5657,7 @@
         <v>85203</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A63" s="7">
         <v>43891</v>
       </c>
@@ -4699,7 +5665,7 @@
         <v>87026</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A64" s="7">
         <v>43892</v>
       </c>
@@ -4707,7 +5673,7 @@
         <v>89068</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A65" s="7">
         <v>43893</v>
       </c>
@@ -4715,7 +5681,7 @@
         <v>90865</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A66" s="7">
         <v>43894</v>
       </c>
@@ -4723,7 +5689,7 @@
         <v>93077</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A67" s="7">
         <v>43895</v>
       </c>
@@ -4731,7 +5697,7 @@
         <v>95316</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A68" s="7">
         <v>43896</v>
       </c>
@@ -4739,7 +5705,7 @@
         <v>98172</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A69" s="7">
         <v>43897</v>
       </c>
@@ -4747,7 +5713,7 @@
         <v>102133</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A70" s="7">
         <v>43898</v>
       </c>
@@ -4755,7 +5721,7 @@
         <v>105824</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A71" s="7">
         <v>43899</v>
       </c>
@@ -4763,7 +5729,7 @@
         <v>109695</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A72" s="7">
         <v>43900</v>
       </c>
@@ -4771,7 +5737,7 @@
         <v>114235</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A73" s="7">
         <v>43901</v>
       </c>
@@ -4779,7 +5745,7 @@
         <v>118613</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A74" s="7">
         <v>43902</v>
       </c>
@@ -4787,7 +5753,7 @@
         <v>125497</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A75" s="7">
         <v>43903</v>
       </c>
@@ -4795,7 +5761,7 @@
         <v>133853</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A76" s="7">
         <v>43904</v>
       </c>
@@ -4803,7 +5769,7 @@
         <v>143259</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A77" s="7">
         <v>43905</v>
       </c>
@@ -4811,7 +5777,7 @@
         <v>154774</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A78" s="7">
         <v>43906</v>
       </c>
@@ -4819,7 +5785,7 @@
         <v>167418</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A79" s="7">
         <v>43907</v>
       </c>
@@ -4827,7 +5793,7 @@
         <v>180094</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A80" s="7">
         <v>43908</v>
       </c>
@@ -4835,7 +5801,7 @@
         <v>194843</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A81" s="7">
         <v>43909</v>
       </c>
@@ -4843,7 +5809,7 @@
         <v>213149</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A82" s="7">
         <v>43910</v>
       </c>
@@ -4851,7 +5817,7 @@
         <v>242374</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A83" s="7">
         <v>43911</v>
       </c>
@@ -4859,7 +5825,7 @@
         <v>271116</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A84" s="7">
         <v>43912</v>
       </c>
@@ -4867,7 +5833,7 @@
         <v>305235</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A85" s="7">
         <v>43913</v>
       </c>
@@ -4875,7 +5841,7 @@
         <v>338235</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A86" s="7">
         <v>43914</v>
       </c>
@@ -4883,7 +5849,7 @@
         <v>377968</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A87" s="7">
         <v>43915</v>
       </c>
@@ -4891,7 +5857,7 @@
         <v>416881</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A88" s="7">
         <v>43916</v>
       </c>
@@ -4899,7 +5865,7 @@
         <v>468092</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A89" s="7">
         <v>43917</v>
       </c>
@@ -4907,7 +5873,7 @@
         <v>527839</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A90" s="7">
         <v>43918</v>
       </c>
@@ -4915,7 +5881,7 @@
         <v>591796</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A91" s="7">
         <v>43919</v>
       </c>
@@ -4923,7 +5889,7 @@
         <v>656834</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A92" s="7">
         <v>43920</v>
       </c>
@@ -4931,7 +5897,7 @@
         <v>715377</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A93" s="7">
         <v>43921</v>
       </c>
@@ -4939,7 +5905,7 @@
         <v>777187</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A94" s="7">
         <v>43922</v>
       </c>
@@ -4947,7 +5913,7 @@
         <v>851587</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A95" s="7">
         <v>43923</v>
       </c>
@@ -4955,7 +5921,7 @@
         <v>928491</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A96" s="7">
         <v>43924</v>
       </c>
@@ -4963,7 +5929,7 @@
         <v>1006063</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A97" s="7">
         <v>43925</v>
       </c>
@@ -4971,7 +5937,7 @@
         <v>1087822</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A98" s="7">
         <v>43926</v>
       </c>
@@ -4979,7 +5945,7 @@
         <v>1174306</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A99" s="7">
         <v>43927</v>
       </c>
@@ -4987,7 +5953,7 @@
         <v>1245601</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A100" s="7">
         <v>43928</v>
       </c>
@@ -4995,7 +5961,7 @@
         <v>1316988</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A101" s="7">
         <v>43929</v>
       </c>
@@ -5003,7 +5969,7 @@
         <v>1391881</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A102" s="7">
         <v>43930</v>
       </c>
@@ -5011,7 +5977,7 @@
         <v>1476792</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A103" s="7">
         <v>43931</v>
       </c>
@@ -5019,7 +5985,7 @@
         <v>1563819</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A104" s="7">
         <v>43932</v>
       </c>
@@ -5027,7 +5993,7 @@
         <v>1653160</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A105" s="7">
         <v>43933</v>
       </c>
@@ -5035,7 +6001,7 @@
         <v>1734868</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A106" s="7">
         <v>43934</v>
       </c>
@@ -5043,7 +6009,7 @@
         <v>1807256</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A107" s="7">
         <v>43935</v>
       </c>
@@ -5051,7 +6017,7 @@
         <v>1873639</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A108" s="7">
         <v>43936</v>
       </c>
@@ -5059,7 +6025,7 @@
         <v>1953786</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A109" s="7">
         <v>43937</v>
       </c>
@@ -5067,7 +6033,7 @@
         <v>2033745</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A110" s="7">
         <v>43938</v>
       </c>
@@ -5075,7 +6041,7 @@
         <v>2117297</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A111" s="7">
         <v>43939</v>
       </c>
@@ -5083,7 +6049,7 @@
         <v>2199460</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A112" s="7">
         <v>43940</v>
       </c>
@@ -5091,7 +6057,7 @@
         <v>2278484</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A113" s="7">
         <v>43941</v>
       </c>
@@ -5099,7 +6065,7 @@
         <v>2350993</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A114" s="7">
         <v>43942</v>
       </c>
@@ -5107,7 +6073,7 @@
         <v>2427353</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A115" s="7">
         <v>43943</v>
       </c>
@@ -5115,7 +6081,7 @@
         <v>2513399</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A116" s="7">
         <v>43944</v>
       </c>
@@ -5123,7 +6089,7 @@
         <v>2579823</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A117" s="7">
         <v>43945</v>
       </c>
@@ -5131,7 +6097,7 @@
         <v>2657910</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A118" s="7">
         <v>43946</v>
       </c>
@@ -5139,7 +6105,7 @@
         <v>2730743</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A119" s="7">
         <v>43947</v>
       </c>
@@ -5147,7 +6113,7 @@
         <v>2832459</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A120" s="7">
         <v>43948</v>
       </c>
@@ -5155,7 +6121,7 @@
         <v>2915995</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A121" s="7">
         <v>43949</v>
       </c>
@@ -5163,7 +6129,7 @@
         <v>2981427</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A122" s="7">
         <v>43950</v>
       </c>
@@ -5171,7 +6137,7 @@
         <v>3054404</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A123" s="7">
         <v>43951</v>
       </c>
@@ -5179,7 +6145,7 @@
         <v>3131302</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A124" s="7">
         <v>43952</v>
       </c>
@@ -5187,7 +6153,7 @@
         <v>3216031</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A125" s="7">
         <v>43953</v>
       </c>
@@ -5195,7 +6161,7 @@
         <v>3308966</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A126" s="7">
         <v>43954</v>
       </c>
@@ -5203,7 +6169,7 @@
         <v>3389549</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A127" s="7">
         <v>43955</v>
       </c>
@@ -5212,7 +6178,227 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125F9AE1-2C98-413C-9729-A847C95170BD}">
+  <dimension ref="A1:P16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>2005</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1927</v>
+      </c>
+      <c r="C2" s="8">
+        <f>B2/1000</f>
+        <v>1.927</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>2006</v>
+      </c>
+      <c r="B3" s="8">
+        <v>3675</v>
+      </c>
+      <c r="C3" s="8">
+        <f t="shared" ref="C3:C16" si="0">B3/1000</f>
+        <v>3.6749999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>2007</v>
+      </c>
+      <c r="B4" s="8">
+        <v>5710</v>
+      </c>
+      <c r="C4" s="8">
+        <f t="shared" si="0"/>
+        <v>5.71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>2008</v>
+      </c>
+      <c r="B5" s="8">
+        <v>14800</v>
+      </c>
+      <c r="C5" s="8">
+        <f t="shared" si="0"/>
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>2009</v>
+      </c>
+      <c r="B6" s="8">
+        <v>26900</v>
+      </c>
+      <c r="C6" s="8">
+        <f t="shared" si="0"/>
+        <v>26.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>2010</v>
+      </c>
+      <c r="B7" s="8">
+        <v>44622</v>
+      </c>
+      <c r="C7" s="8">
+        <f t="shared" si="0"/>
+        <v>44.622</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>2011</v>
+      </c>
+      <c r="B8" s="8">
+        <v>74100</v>
+      </c>
+      <c r="C8" s="8">
+        <f t="shared" si="0"/>
+        <v>74.099999999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>2012</v>
+      </c>
+      <c r="B9" s="8">
+        <v>103000</v>
+      </c>
+      <c r="C9" s="8">
+        <f t="shared" si="0"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>2013</v>
+      </c>
+      <c r="B10" s="8">
+        <v>134900</v>
+      </c>
+      <c r="C10" s="8">
+        <f t="shared" si="0"/>
+        <v>134.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>2014</v>
+      </c>
+      <c r="B11" s="8">
+        <v>153400</v>
+      </c>
+      <c r="C11" s="8">
+        <f t="shared" si="0"/>
+        <v>153.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>2015</v>
+      </c>
+      <c r="B12" s="8">
+        <v>186300</v>
+      </c>
+      <c r="C12" s="8">
+        <f t="shared" si="0"/>
+        <v>186.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>2016</v>
+      </c>
+      <c r="B13" s="8">
+        <v>241000</v>
+      </c>
+      <c r="C13" s="8">
+        <f t="shared" si="0"/>
+        <v>241</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>2017</v>
+      </c>
+      <c r="B14" s="8">
+        <v>305700</v>
+      </c>
+      <c r="C14" s="8">
+        <f t="shared" si="0"/>
+        <v>305.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>2018</v>
+      </c>
+      <c r="B15" s="8">
+        <v>366000</v>
+      </c>
+      <c r="C15" s="8">
+        <f t="shared" si="0"/>
+        <v>366</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>2019</v>
+      </c>
+      <c r="B16" s="8">
+        <v>405700</v>
+      </c>
+      <c r="C16" s="8">
+        <f t="shared" si="0"/>
+        <v>405.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>